<commit_message>
apply the COUNTIF and SUMIF formulas
</commit_message>
<xml_diff>
--- a/Kitchen Supplies-Transaction.xlsx
+++ b/Kitchen Supplies-Transaction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>ID Transaksi</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>QUESTION :</t>
+  </si>
+  <si>
+    <t>ANSWER</t>
   </si>
   <si>
     <t>Berapa banyak transaksi yang hanya berisi 1 barang?</t>
@@ -55,9 +58,6 @@
     <t>Pendapatan rata-rata per transaksi</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>&gt;1</t>
   </si>
 </sst>
@@ -66,14 +66,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="181" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -83,6 +83,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
@@ -102,7 +109,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -117,30 +147,31 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,48 +185,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,44 +231,28 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,31 +267,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,151 +453,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,15 +512,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -517,6 +527,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -528,15 +547,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,176 +591,198 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1017,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1041,9 +1073,11 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" customHeight="1" spans="1:5">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="4">
         <v>123</v>
       </c>
@@ -1054,7 +1088,10 @@
         <v>100</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F3" s="7">
+        <v>25</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
@@ -1068,9 +1105,11 @@
         <v>120</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="F4" s="8">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="4">
@@ -1083,9 +1122,11 @@
         <v>110</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1555</v>
+      </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="4">
@@ -1098,9 +1139,11 @@
         <v>80</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F6" s="9">
+        <v>4735</v>
+      </c>
     </row>
     <row r="7" customHeight="1" spans="1:6">
       <c r="A7" s="4">
@@ -1113,11 +1156,13 @@
         <v>400</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" customHeight="1" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F7" s="9">
+        <v>62.2</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="4">
         <v>128</v>
       </c>
@@ -1128,7 +1173,10 @@
         <v>90</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="10">
+        <v>205.869565217391</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:3">
@@ -1152,17 +1200,17 @@
       <c r="C10" s="5">
         <v>70</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="H10" s="11" t="s">
         <v>12</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:9">
@@ -1175,15 +1223,20 @@
       <c r="C11" s="5">
         <v>540</v>
       </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>13</v>
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12">
+        <f>COUNTIF($B$3:$B$50,"=1")</f>
+        <v>25</v>
+      </c>
+      <c r="H11" s="13">
+        <f>SUMIF($B$3:$B$50,"=1",$C$3:$C$50)</f>
+        <v>1555</v>
+      </c>
+      <c r="I11" s="13">
+        <f>H11/G11</f>
+        <v>62.2</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:9">
@@ -1196,15 +1249,20 @@
       <c r="C12" s="5">
         <v>100</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>13</v>
+      <c r="G12" s="12">
+        <f>COUNTIF($B$3:$B$50,"&gt;1")</f>
+        <v>23</v>
+      </c>
+      <c r="H12" s="13">
+        <f>SUMIF($B$3:$B$50,"&gt;1",$C$3:$C$50)</f>
+        <v>4735</v>
+      </c>
+      <c r="I12" s="13">
+        <f>H12/G12</f>
+        <v>205.869565217391</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:3">

</xml_diff>